<commit_message>
browser headless is activated
</commit_message>
<xml_diff>
--- a/testresult.xlsx
+++ b/testresult.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5645" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5929" uniqueCount="301">
   <si>
     <t>S.No</t>
   </si>
@@ -883,6 +883,60 @@
   </si>
   <si>
     <t>https://www.naukri.com/job-listings-qa-tester-lead-tekgence-pune-chennai-6-to-10-years-130126031914</t>
+  </si>
+  <si>
+    <t>Automation Test Engineer (UFT)</t>
+  </si>
+  <si>
+    <t>https://www.naukri.com/job-listings-automation-test-engineer-uft-tata-consultancy-services-chennai-bengaluru-5-to-10-years-080126026105</t>
+  </si>
+  <si>
+    <t>Automation Testing Engineer- Playwright</t>
+  </si>
+  <si>
+    <t>https://www.naukri.com/job-listings-automation-testing-engineer-playwright-sonata-software-hyderabad-chennai-bengaluru-7-to-12-years-231225035819</t>
+  </si>
+  <si>
+    <t>Automation Test Engineer(C#+API)</t>
+  </si>
+  <si>
+    <t>https://www.naukri.com/job-listings-automation-test-engineer-c-api-ltimindtree-hyderabad-chennai-bengaluru-5-to-10-years-020126008100</t>
+  </si>
+  <si>
+    <t>https://www.naukri.com/job-listings-test-automation-engineer-accenture-solutions-pvt-ltd-chennai-3-to-8-years-130126921557</t>
+  </si>
+  <si>
+    <t>Storage Test Automation Engineer</t>
+  </si>
+  <si>
+    <t>https://www.naukri.com/job-listings-storage-test-automation-engineer-aziro-pune-chennai-bengaluru-4-to-9-years-110126008534</t>
+  </si>
+  <si>
+    <t>Cypress Automation Test Engineer</t>
+  </si>
+  <si>
+    <t>https://www.naukri.com/job-listings-cypress-automation-test-engineer-cognizant-chennai-4-to-10-years-020126013272</t>
+  </si>
+  <si>
+    <t>Test Automation Engineer | Contract</t>
+  </si>
+  <si>
+    <t>https://www.naukri.com/job-listings-test-automation-engineer-contract-srs-infoway-chennai-8-to-10-years-090126939555</t>
+  </si>
+  <si>
+    <t>IVI Test Automation Engineer (Automotive Infotainment)</t>
+  </si>
+  <si>
+    <t>https://www.naukri.com/job-listings-ivi-test-automation-engineer-automotive-infotainment-tekpillar-pune-chennai-bengaluru-5-to-10-years-100126000791</t>
+  </si>
+  <si>
+    <t>IVR Automation Test Engineer(Cyara &amp; Kore.ai)</t>
+  </si>
+  <si>
+    <t>https://www.naukri.com/job-listings-ivr-automation-test-engineer-cyara-kore-ai-summitworks-technologies-pune-chennai-5-to-10-years-030126013225</t>
+  </si>
+  <si>
+    <t>https://www.naukri.com/job-listings-automation-test-engineer-indium-software-chennai-bengaluru-5-to-10-years-090126019771</t>
   </si>
 </sst>
 </file>
@@ -957,7 +1011,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E1411"/>
+  <dimension ref="A1:E1482"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -24957,6 +25011,1213 @@
         <v>8</v>
       </c>
     </row>
+    <row r="1412">
+      <c r="A1412" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="B1412" t="s" s="0">
+        <v>283</v>
+      </c>
+      <c r="C1412" t="s" s="0">
+        <v>284</v>
+      </c>
+      <c r="D1412" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="E1412" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1413">
+      <c r="A1413" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="B1413" t="s" s="0">
+        <v>285</v>
+      </c>
+      <c r="C1413" t="s" s="0">
+        <v>286</v>
+      </c>
+      <c r="D1413" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="E1413" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1414">
+      <c r="A1414" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="B1414" t="s" s="0">
+        <v>287</v>
+      </c>
+      <c r="C1414" t="s" s="0">
+        <v>288</v>
+      </c>
+      <c r="D1414" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="E1414" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1415">
+      <c r="A1415" t="n" s="0">
+        <v>4.0</v>
+      </c>
+      <c r="B1415" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C1415" t="s" s="0">
+        <v>289</v>
+      </c>
+      <c r="D1415" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="E1415" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1416">
+      <c r="A1416" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="B1416" t="s" s="0">
+        <v>290</v>
+      </c>
+      <c r="C1416" t="s" s="0">
+        <v>291</v>
+      </c>
+      <c r="D1416" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="E1416" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1417">
+      <c r="A1417" t="n" s="0">
+        <v>6.0</v>
+      </c>
+      <c r="B1417" t="s" s="0">
+        <v>292</v>
+      </c>
+      <c r="C1417" t="s" s="0">
+        <v>293</v>
+      </c>
+      <c r="D1417" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="E1417" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1418">
+      <c r="A1418" t="n" s="0">
+        <v>7.0</v>
+      </c>
+      <c r="B1418" t="s" s="0">
+        <v>294</v>
+      </c>
+      <c r="C1418" t="s" s="0">
+        <v>295</v>
+      </c>
+      <c r="D1418" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="E1418" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1419">
+      <c r="A1419" t="n" s="0">
+        <v>8.0</v>
+      </c>
+      <c r="B1419" t="s" s="0">
+        <v>296</v>
+      </c>
+      <c r="C1419" t="s" s="0">
+        <v>297</v>
+      </c>
+      <c r="D1419" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="E1419" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1420">
+      <c r="A1420" t="n" s="0">
+        <v>9.0</v>
+      </c>
+      <c r="B1420" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C1420" t="s" s="0">
+        <v>299</v>
+      </c>
+      <c r="D1420" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="E1420" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1421">
+      <c r="A1421" t="n" s="0">
+        <v>10.0</v>
+      </c>
+      <c r="B1421" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C1421" t="s" s="0">
+        <v>300</v>
+      </c>
+      <c r="D1421" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="E1421" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1422">
+      <c r="A1422" t="n" s="0">
+        <v>11.0</v>
+      </c>
+      <c r="B1422" t="s" s="0">
+        <v>283</v>
+      </c>
+      <c r="C1422" t="s" s="0">
+        <v>284</v>
+      </c>
+      <c r="D1422" t="s" s="0">
+        <v>241</v>
+      </c>
+      <c r="E1422" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1423">
+      <c r="A1423" t="n" s="0">
+        <v>12.0</v>
+      </c>
+      <c r="B1423" t="s" s="0">
+        <v>285</v>
+      </c>
+      <c r="C1423" t="s" s="0">
+        <v>286</v>
+      </c>
+      <c r="D1423" t="s" s="0">
+        <v>241</v>
+      </c>
+      <c r="E1423" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1424">
+      <c r="A1424" t="n" s="0">
+        <v>13.0</v>
+      </c>
+      <c r="B1424" t="s" s="0">
+        <v>287</v>
+      </c>
+      <c r="C1424" t="s" s="0">
+        <v>288</v>
+      </c>
+      <c r="D1424" t="s" s="0">
+        <v>241</v>
+      </c>
+      <c r="E1424" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1425">
+      <c r="A1425" t="n" s="0">
+        <v>14.0</v>
+      </c>
+      <c r="B1425" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C1425" t="s" s="0">
+        <v>289</v>
+      </c>
+      <c r="D1425" t="s" s="0">
+        <v>241</v>
+      </c>
+      <c r="E1425" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1426">
+      <c r="A1426" t="n" s="0">
+        <v>15.0</v>
+      </c>
+      <c r="B1426" t="s" s="0">
+        <v>290</v>
+      </c>
+      <c r="C1426" t="s" s="0">
+        <v>291</v>
+      </c>
+      <c r="D1426" t="s" s="0">
+        <v>241</v>
+      </c>
+      <c r="E1426" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1427">
+      <c r="A1427" t="n" s="0">
+        <v>16.0</v>
+      </c>
+      <c r="B1427" t="s" s="0">
+        <v>292</v>
+      </c>
+      <c r="C1427" t="s" s="0">
+        <v>293</v>
+      </c>
+      <c r="D1427" t="s" s="0">
+        <v>241</v>
+      </c>
+      <c r="E1427" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1428">
+      <c r="A1428" t="n" s="0">
+        <v>17.0</v>
+      </c>
+      <c r="B1428" t="s" s="0">
+        <v>294</v>
+      </c>
+      <c r="C1428" t="s" s="0">
+        <v>295</v>
+      </c>
+      <c r="D1428" t="s" s="0">
+        <v>241</v>
+      </c>
+      <c r="E1428" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1429">
+      <c r="A1429" t="n" s="0">
+        <v>18.0</v>
+      </c>
+      <c r="B1429" t="s" s="0">
+        <v>296</v>
+      </c>
+      <c r="C1429" t="s" s="0">
+        <v>297</v>
+      </c>
+      <c r="D1429" t="s" s="0">
+        <v>241</v>
+      </c>
+      <c r="E1429" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1430">
+      <c r="A1430" t="n" s="0">
+        <v>19.0</v>
+      </c>
+      <c r="B1430" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C1430" t="s" s="0">
+        <v>299</v>
+      </c>
+      <c r="D1430" t="s" s="0">
+        <v>241</v>
+      </c>
+      <c r="E1430" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1431">
+      <c r="A1431" t="n" s="0">
+        <v>20.0</v>
+      </c>
+      <c r="B1431" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C1431" t="s" s="0">
+        <v>300</v>
+      </c>
+      <c r="D1431" t="s" s="0">
+        <v>241</v>
+      </c>
+      <c r="E1431" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1432">
+      <c r="A1432" t="n" s="0">
+        <v>21.0</v>
+      </c>
+      <c r="B1432" t="s" s="0">
+        <v>283</v>
+      </c>
+      <c r="C1432" t="s" s="0">
+        <v>284</v>
+      </c>
+      <c r="D1432" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E1432" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1433">
+      <c r="A1433" t="n" s="0">
+        <v>22.0</v>
+      </c>
+      <c r="B1433" t="s" s="0">
+        <v>285</v>
+      </c>
+      <c r="C1433" t="s" s="0">
+        <v>286</v>
+      </c>
+      <c r="D1433" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E1433" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1434">
+      <c r="A1434" t="n" s="0">
+        <v>23.0</v>
+      </c>
+      <c r="B1434" t="s" s="0">
+        <v>287</v>
+      </c>
+      <c r="C1434" t="s" s="0">
+        <v>288</v>
+      </c>
+      <c r="D1434" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E1434" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1435">
+      <c r="A1435" t="n" s="0">
+        <v>24.0</v>
+      </c>
+      <c r="B1435" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C1435" t="s" s="0">
+        <v>289</v>
+      </c>
+      <c r="D1435" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E1435" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1436">
+      <c r="A1436" t="n" s="0">
+        <v>25.0</v>
+      </c>
+      <c r="B1436" t="s" s="0">
+        <v>290</v>
+      </c>
+      <c r="C1436" t="s" s="0">
+        <v>291</v>
+      </c>
+      <c r="D1436" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E1436" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1437">
+      <c r="A1437" t="n" s="0">
+        <v>26.0</v>
+      </c>
+      <c r="B1437" t="s" s="0">
+        <v>292</v>
+      </c>
+      <c r="C1437" t="s" s="0">
+        <v>293</v>
+      </c>
+      <c r="D1437" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E1437" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1438">
+      <c r="A1438" t="n" s="0">
+        <v>27.0</v>
+      </c>
+      <c r="B1438" t="s" s="0">
+        <v>294</v>
+      </c>
+      <c r="C1438" t="s" s="0">
+        <v>295</v>
+      </c>
+      <c r="D1438" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E1438" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1439">
+      <c r="A1439" t="n" s="0">
+        <v>28.0</v>
+      </c>
+      <c r="B1439" t="s" s="0">
+        <v>296</v>
+      </c>
+      <c r="C1439" t="s" s="0">
+        <v>297</v>
+      </c>
+      <c r="D1439" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E1439" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1440">
+      <c r="A1440" t="n" s="0">
+        <v>29.0</v>
+      </c>
+      <c r="B1440" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C1440" t="s" s="0">
+        <v>299</v>
+      </c>
+      <c r="D1440" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E1440" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1441">
+      <c r="A1441" t="n" s="0">
+        <v>30.0</v>
+      </c>
+      <c r="B1441" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C1441" t="s" s="0">
+        <v>300</v>
+      </c>
+      <c r="D1441" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E1441" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1442">
+      <c r="A1442" t="n" s="0">
+        <v>31.0</v>
+      </c>
+      <c r="B1442" t="s" s="0">
+        <v>283</v>
+      </c>
+      <c r="C1442" t="s" s="0">
+        <v>284</v>
+      </c>
+      <c r="D1442" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="E1442" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1443">
+      <c r="A1443" t="n" s="0">
+        <v>32.0</v>
+      </c>
+      <c r="B1443" t="s" s="0">
+        <v>285</v>
+      </c>
+      <c r="C1443" t="s" s="0">
+        <v>286</v>
+      </c>
+      <c r="D1443" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="E1443" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1444">
+      <c r="A1444" t="n" s="0">
+        <v>33.0</v>
+      </c>
+      <c r="B1444" t="s" s="0">
+        <v>287</v>
+      </c>
+      <c r="C1444" t="s" s="0">
+        <v>288</v>
+      </c>
+      <c r="D1444" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="E1444" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1445">
+      <c r="A1445" t="n" s="0">
+        <v>34.0</v>
+      </c>
+      <c r="B1445" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C1445" t="s" s="0">
+        <v>289</v>
+      </c>
+      <c r="D1445" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="E1445" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1446">
+      <c r="A1446" t="n" s="0">
+        <v>35.0</v>
+      </c>
+      <c r="B1446" t="s" s="0">
+        <v>290</v>
+      </c>
+      <c r="C1446" t="s" s="0">
+        <v>291</v>
+      </c>
+      <c r="D1446" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="E1446" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1447">
+      <c r="A1447" t="n" s="0">
+        <v>36.0</v>
+      </c>
+      <c r="B1447" t="s" s="0">
+        <v>292</v>
+      </c>
+      <c r="C1447" t="s" s="0">
+        <v>293</v>
+      </c>
+      <c r="D1447" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="E1447" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1448">
+      <c r="A1448" t="n" s="0">
+        <v>37.0</v>
+      </c>
+      <c r="B1448" t="s" s="0">
+        <v>294</v>
+      </c>
+      <c r="C1448" t="s" s="0">
+        <v>295</v>
+      </c>
+      <c r="D1448" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="E1448" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1449">
+      <c r="A1449" t="n" s="0">
+        <v>38.0</v>
+      </c>
+      <c r="B1449" t="s" s="0">
+        <v>296</v>
+      </c>
+      <c r="C1449" t="s" s="0">
+        <v>297</v>
+      </c>
+      <c r="D1449" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="E1449" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1450">
+      <c r="A1450" t="n" s="0">
+        <v>39.0</v>
+      </c>
+      <c r="B1450" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C1450" t="s" s="0">
+        <v>299</v>
+      </c>
+      <c r="D1450" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="E1450" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1451">
+      <c r="A1451" t="n" s="0">
+        <v>40.0</v>
+      </c>
+      <c r="B1451" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C1451" t="s" s="0">
+        <v>300</v>
+      </c>
+      <c r="D1451" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="E1451" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1452">
+      <c r="A1452" t="n" s="0">
+        <v>41.0</v>
+      </c>
+      <c r="B1452" t="s" s="0">
+        <v>283</v>
+      </c>
+      <c r="C1452" t="s" s="0">
+        <v>284</v>
+      </c>
+      <c r="D1452" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="E1452" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1453">
+      <c r="A1453" t="n" s="0">
+        <v>42.0</v>
+      </c>
+      <c r="B1453" t="s" s="0">
+        <v>285</v>
+      </c>
+      <c r="C1453" t="s" s="0">
+        <v>286</v>
+      </c>
+      <c r="D1453" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="E1453" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1454">
+      <c r="A1454" t="n" s="0">
+        <v>43.0</v>
+      </c>
+      <c r="B1454" t="s" s="0">
+        <v>287</v>
+      </c>
+      <c r="C1454" t="s" s="0">
+        <v>288</v>
+      </c>
+      <c r="D1454" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="E1454" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1455">
+      <c r="A1455" t="n" s="0">
+        <v>44.0</v>
+      </c>
+      <c r="B1455" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C1455" t="s" s="0">
+        <v>289</v>
+      </c>
+      <c r="D1455" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="E1455" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1456">
+      <c r="A1456" t="n" s="0">
+        <v>45.0</v>
+      </c>
+      <c r="B1456" t="s" s="0">
+        <v>290</v>
+      </c>
+      <c r="C1456" t="s" s="0">
+        <v>291</v>
+      </c>
+      <c r="D1456" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="E1456" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1457">
+      <c r="A1457" t="n" s="0">
+        <v>46.0</v>
+      </c>
+      <c r="B1457" t="s" s="0">
+        <v>292</v>
+      </c>
+      <c r="C1457" t="s" s="0">
+        <v>293</v>
+      </c>
+      <c r="D1457" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="E1457" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1458">
+      <c r="A1458" t="n" s="0">
+        <v>47.0</v>
+      </c>
+      <c r="B1458" t="s" s="0">
+        <v>294</v>
+      </c>
+      <c r="C1458" t="s" s="0">
+        <v>295</v>
+      </c>
+      <c r="D1458" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="E1458" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1459">
+      <c r="A1459" t="n" s="0">
+        <v>48.0</v>
+      </c>
+      <c r="B1459" t="s" s="0">
+        <v>296</v>
+      </c>
+      <c r="C1459" t="s" s="0">
+        <v>297</v>
+      </c>
+      <c r="D1459" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="E1459" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1460">
+      <c r="A1460" t="n" s="0">
+        <v>49.0</v>
+      </c>
+      <c r="B1460" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C1460" t="s" s="0">
+        <v>299</v>
+      </c>
+      <c r="D1460" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="E1460" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1461">
+      <c r="A1461" t="n" s="0">
+        <v>50.0</v>
+      </c>
+      <c r="B1461" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C1461" t="s" s="0">
+        <v>300</v>
+      </c>
+      <c r="D1461" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="E1461" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1462">
+      <c r="A1462" t="n" s="0">
+        <v>51.0</v>
+      </c>
+      <c r="B1462" t="s" s="0">
+        <v>283</v>
+      </c>
+      <c r="C1462" t="s" s="0">
+        <v>284</v>
+      </c>
+      <c r="D1462" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="E1462" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1463">
+      <c r="A1463" t="n" s="0">
+        <v>52.0</v>
+      </c>
+      <c r="B1463" t="s" s="0">
+        <v>285</v>
+      </c>
+      <c r="C1463" t="s" s="0">
+        <v>286</v>
+      </c>
+      <c r="D1463" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="E1463" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1464">
+      <c r="A1464" t="n" s="0">
+        <v>53.0</v>
+      </c>
+      <c r="B1464" t="s" s="0">
+        <v>287</v>
+      </c>
+      <c r="C1464" t="s" s="0">
+        <v>288</v>
+      </c>
+      <c r="D1464" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="E1464" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1465">
+      <c r="A1465" t="n" s="0">
+        <v>54.0</v>
+      </c>
+      <c r="B1465" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C1465" t="s" s="0">
+        <v>289</v>
+      </c>
+      <c r="D1465" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="E1465" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1466">
+      <c r="A1466" t="n" s="0">
+        <v>55.0</v>
+      </c>
+      <c r="B1466" t="s" s="0">
+        <v>290</v>
+      </c>
+      <c r="C1466" t="s" s="0">
+        <v>291</v>
+      </c>
+      <c r="D1466" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="E1466" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1467">
+      <c r="A1467" t="n" s="0">
+        <v>56.0</v>
+      </c>
+      <c r="B1467" t="s" s="0">
+        <v>292</v>
+      </c>
+      <c r="C1467" t="s" s="0">
+        <v>293</v>
+      </c>
+      <c r="D1467" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="E1467" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1468">
+      <c r="A1468" t="n" s="0">
+        <v>57.0</v>
+      </c>
+      <c r="B1468" t="s" s="0">
+        <v>294</v>
+      </c>
+      <c r="C1468" t="s" s="0">
+        <v>295</v>
+      </c>
+      <c r="D1468" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="E1468" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1469">
+      <c r="A1469" t="n" s="0">
+        <v>58.0</v>
+      </c>
+      <c r="B1469" t="s" s="0">
+        <v>296</v>
+      </c>
+      <c r="C1469" t="s" s="0">
+        <v>297</v>
+      </c>
+      <c r="D1469" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="E1469" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1470">
+      <c r="A1470" t="n" s="0">
+        <v>59.0</v>
+      </c>
+      <c r="B1470" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C1470" t="s" s="0">
+        <v>299</v>
+      </c>
+      <c r="D1470" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="E1470" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1471">
+      <c r="A1471" t="n" s="0">
+        <v>60.0</v>
+      </c>
+      <c r="B1471" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C1471" t="s" s="0">
+        <v>300</v>
+      </c>
+      <c r="D1471" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="E1471" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1472">
+      <c r="A1472" t="n" s="0">
+        <v>61.0</v>
+      </c>
+      <c r="B1472" t="s" s="0">
+        <v>283</v>
+      </c>
+      <c r="C1472" t="s" s="0">
+        <v>284</v>
+      </c>
+      <c r="D1472" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="E1472" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1473">
+      <c r="A1473" t="n" s="0">
+        <v>62.0</v>
+      </c>
+      <c r="B1473" t="s" s="0">
+        <v>285</v>
+      </c>
+      <c r="C1473" t="s" s="0">
+        <v>286</v>
+      </c>
+      <c r="D1473" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="E1473" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1474">
+      <c r="A1474" t="n" s="0">
+        <v>63.0</v>
+      </c>
+      <c r="B1474" t="s" s="0">
+        <v>287</v>
+      </c>
+      <c r="C1474" t="s" s="0">
+        <v>288</v>
+      </c>
+      <c r="D1474" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="E1474" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1475">
+      <c r="A1475" t="n" s="0">
+        <v>64.0</v>
+      </c>
+      <c r="B1475" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C1475" t="s" s="0">
+        <v>289</v>
+      </c>
+      <c r="D1475" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="E1475" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1476">
+      <c r="A1476" t="n" s="0">
+        <v>65.0</v>
+      </c>
+      <c r="B1476" t="s" s="0">
+        <v>290</v>
+      </c>
+      <c r="C1476" t="s" s="0">
+        <v>291</v>
+      </c>
+      <c r="D1476" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="E1476" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1477">
+      <c r="A1477" t="n" s="0">
+        <v>66.0</v>
+      </c>
+      <c r="B1477" t="s" s="0">
+        <v>292</v>
+      </c>
+      <c r="C1477" t="s" s="0">
+        <v>293</v>
+      </c>
+      <c r="D1477" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="E1477" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1478">
+      <c r="A1478" t="n" s="0">
+        <v>67.0</v>
+      </c>
+      <c r="B1478" t="s" s="0">
+        <v>294</v>
+      </c>
+      <c r="C1478" t="s" s="0">
+        <v>295</v>
+      </c>
+      <c r="D1478" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="E1478" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1479">
+      <c r="A1479" t="n" s="0">
+        <v>68.0</v>
+      </c>
+      <c r="B1479" t="s" s="0">
+        <v>296</v>
+      </c>
+      <c r="C1479" t="s" s="0">
+        <v>297</v>
+      </c>
+      <c r="D1479" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="E1479" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1480">
+      <c r="A1480" t="n" s="0">
+        <v>69.0</v>
+      </c>
+      <c r="B1480" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C1480" t="s" s="0">
+        <v>299</v>
+      </c>
+      <c r="D1480" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="E1480" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1481">
+      <c r="A1481" t="n" s="0">
+        <v>70.0</v>
+      </c>
+      <c r="B1481" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C1481" t="s" s="0">
+        <v>300</v>
+      </c>
+      <c r="D1481" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="E1481" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1482">
+      <c r="A1482" t="n" s="0">
+        <v>71.0</v>
+      </c>
+      <c r="B1482" t="s" s="0">
+        <v>283</v>
+      </c>
+      <c r="C1482" t="s" s="0">
+        <v>284</v>
+      </c>
+      <c r="D1482" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="E1482" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>